<commit_message>
Operation Chaining 7ns vivado report aggiornati
</commit_message>
<xml_diff>
--- a/reports/vivado/OperationChaining7nsSolution/power/OperationChaining7nsClockEnablePowerReport.xlsx
+++ b/reports/vivado/OperationChaining7nsSolution/power/OperationChaining7nsClockEnablePowerReport.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="27">
   <si>
     <t>Utilization</t>
   </si>
@@ -65,40 +65,31 @@
     <t xml:space="preserve">FF </t>
   </si>
   <si>
+    <t>firConvolutionOperationChaining_IP/U0/p_pn_reg_118[31]_i_1_n_0</t>
+  </si>
+  <si>
+    <t>firConvolutionOperationChaining_IP/U0/ce0</t>
+  </si>
+  <si>
     <t>firConvolutionOperationChaining_IP/U0/shiftRegister_U/firConvolutionOpebkb_ram_U/we0</t>
   </si>
   <si>
     <t xml:space="preserve">RAM </t>
   </si>
   <si>
-    <t>firConvolutionOperationChaining_IP/U0/p_pn_reg_118[31]_i_1_n_0</t>
-  </si>
-  <si>
-    <t>firConvolutionOperationChaining_IP/U0/ce0</t>
-  </si>
-  <si>
     <t>firConvolutionOperationChaining_IP/U0/ap_CS_fsm_state8</t>
   </si>
   <si>
+    <t>firConvolutionOperationChaining_IP/U0/ap_CS_fsm_reg_n_0_[6]</t>
+  </si>
+  <si>
     <t>firConvolutionOperationChaining_IP/U0/ap_CS_fsm_reg_n_0_[5]</t>
   </si>
   <si>
-    <t>firConvolutionOperationChaining_IP/U0/ap_CS_fsm_reg_n_0_[6]</t>
-  </si>
-  <si>
     <t>firConvolutionOperationChaining_IP/U0/ce02</t>
   </si>
   <si>
     <t>firConvolutionOperationChaining_IP/U0/ap_CS_fsm_state3</t>
-  </si>
-  <si>
-    <t>firConvolutionOperationChaining_IP/U0/ap_NS_fsm[3]</t>
-  </si>
-  <si>
-    <t>firConvolutionOperationChaining_IP/U0/ap_NS_fsm[8]</t>
-  </si>
-  <si>
-    <t>firConvolutionOperationChaining_IP/U0/ap_NS_fsm[4]</t>
   </si>
   <si>
     <t>firConvolutionOperationChaining_IP/U0/ap_CS_fsm_reg_n_0_[1]</t>
@@ -223,7 +214,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n" s="2">
-        <v>7.411771221086383E-4</v>
+        <v>4.179837997071445E-4</v>
       </c>
       <c r="B2" t="s" s="4">
         <v>8</v>
@@ -249,7 +240,7 @@
     </row>
     <row r="3" outlineLevel="1">
       <c r="A3" t="n" s="5">
-        <v>2.2369612997863442E-4</v>
+        <v>1.023563600028865E-4</v>
       </c>
       <c r="B3" t="s" s="4">
         <v>10</v>
@@ -264,7 +255,7 @@
         <v>105.0</v>
       </c>
       <c r="F3" t="n" s="7">
-        <v>0.0</v>
+        <v>20.0</v>
       </c>
       <c r="G3" t="s" s="4">
         <v>11</v>
@@ -275,7 +266,7 @@
     </row>
     <row r="4" outlineLevel="1">
       <c r="A4" t="n" s="5">
-        <v>1.2101454194635153E-4</v>
+        <v>1.0136581840924919E-4</v>
       </c>
       <c r="B4" t="s" s="4">
         <v>13</v>
@@ -290,7 +281,7 @@
         <v>74.0</v>
       </c>
       <c r="F4" t="n" s="7">
-        <v>0.0</v>
+        <v>28.0</v>
       </c>
       <c r="G4" t="s" s="4">
         <v>11</v>
@@ -301,7 +292,7 @@
     </row>
     <row r="5" outlineLevel="1">
       <c r="A5" t="n" s="5">
-        <v>1.1985292803728953E-4</v>
+        <v>8.802818047115579E-5</v>
       </c>
       <c r="B5" t="s" s="4">
         <v>15</v>
@@ -316,7 +307,7 @@
         <v>32.0</v>
       </c>
       <c r="F5" t="n" s="7">
-        <v>0.0</v>
+        <v>16.0</v>
       </c>
       <c r="G5" t="s" s="4">
         <v>11</v>
@@ -327,85 +318,85 @@
     </row>
     <row r="6" outlineLevel="1">
       <c r="A6" t="n" s="5">
-        <v>6.25647371634841E-5</v>
+        <v>2.899345417972654E-5</v>
       </c>
       <c r="B6" t="s" s="4">
         <v>17</v>
       </c>
       <c r="C6" t="n" s="2">
-        <v>45.272727966308594</v>
+        <v>45.09090805053711</v>
       </c>
       <c r="D6" t="n" s="2">
-        <v>15.80267333984375</v>
+        <v>15.781818389892578</v>
       </c>
       <c r="E6" t="n" s="7">
         <v>32.0</v>
       </c>
       <c r="F6" t="n" s="7">
-        <v>0.0</v>
+        <v>8.0</v>
       </c>
       <c r="G6" t="s" s="4">
         <v>11</v>
       </c>
       <c r="H6" t="s" s="4">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" outlineLevel="1">
       <c r="A7" t="n" s="5">
-        <v>6.231346924323589E-5</v>
+        <v>2.7669817427522503E-5</v>
       </c>
       <c r="B7" t="s" s="4">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" t="n" s="2">
-        <v>45.09090805053711</v>
+        <v>49.45454406738281</v>
       </c>
       <c r="D7" t="n" s="2">
-        <v>15.781818389892578</v>
+        <v>17.30908966064453</v>
       </c>
       <c r="E7" t="n" s="7">
-        <v>32.0</v>
+        <v>18.0</v>
       </c>
       <c r="F7" t="n" s="7">
-        <v>0.0</v>
+        <v>8.0</v>
       </c>
       <c r="G7" t="s" s="4">
         <v>11</v>
       </c>
       <c r="H7" t="s" s="4">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" outlineLevel="1">
       <c r="A8" t="n" s="5">
-        <v>5.7426099374424666E-5</v>
+        <v>2.6801455533131957E-5</v>
       </c>
       <c r="B8" t="s" s="4">
+        <v>19</v>
+      </c>
+      <c r="C8" t="n" s="2">
+        <v>45.272727966308594</v>
+      </c>
+      <c r="D8" t="n" s="2">
+        <v>15.80267333984375</v>
+      </c>
+      <c r="E8" t="n" s="7">
+        <v>32.0</v>
+      </c>
+      <c r="F8" t="n" s="7">
+        <v>8.0</v>
+      </c>
+      <c r="G8" t="s" s="4">
+        <v>11</v>
+      </c>
+      <c r="H8" t="s" s="4">
         <v>20</v>
-      </c>
-      <c r="C8" t="n" s="2">
-        <v>49.45454406738281</v>
-      </c>
-      <c r="D8" t="n" s="2">
-        <v>17.30908966064453</v>
-      </c>
-      <c r="E8" t="n" s="7">
-        <v>18.0</v>
-      </c>
-      <c r="F8" t="n" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="G8" t="s" s="4">
-        <v>11</v>
-      </c>
-      <c r="H8" t="s" s="4">
-        <v>12</v>
       </c>
     </row>
     <row r="9" outlineLevel="1">
       <c r="A9" t="n" s="5">
-        <v>5.7061712141148746E-5</v>
+        <v>2.325745481357444E-5</v>
       </c>
       <c r="B9" t="s" s="4">
         <v>21</v>
@@ -420,7 +411,7 @@
         <v>34.0</v>
       </c>
       <c r="F9" t="n" s="7">
-        <v>0.0</v>
+        <v>7.0</v>
       </c>
       <c r="G9" t="s" s="4">
         <v>11</v>
@@ -431,7 +422,7 @@
     </row>
     <row r="10" outlineLevel="1">
       <c r="A10" t="n" s="5">
-        <v>7.141642981878249E-6</v>
+        <v>6.4512723838561215E-6</v>
       </c>
       <c r="B10" t="s" s="4">
         <v>22</v>
@@ -446,7 +437,7 @@
         <v>2.0</v>
       </c>
       <c r="F10" t="n" s="7">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G10" t="s" s="4">
         <v>11</v>
@@ -457,7 +448,7 @@
     </row>
     <row r="11" outlineLevel="1">
       <c r="A11" t="n" s="5">
-        <v>7.141642981878249E-6</v>
+        <v>5.341817995940801E-6</v>
       </c>
       <c r="B11" t="s" s="4">
         <v>23</v>
@@ -472,7 +463,7 @@
         <v>2.0</v>
       </c>
       <c r="F11" t="n" s="7">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G11" t="s" s="4">
         <v>11</v>
@@ -483,7 +474,7 @@
     </row>
     <row r="12" outlineLevel="1">
       <c r="A12" t="n" s="5">
-        <v>7.025684226391604E-6</v>
+        <v>4.746545073430752E-6</v>
       </c>
       <c r="B12" t="s" s="4">
         <v>24</v>
@@ -498,7 +489,7 @@
         <v>4.0</v>
       </c>
       <c r="F12" t="n" s="7">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G12" t="s" s="4">
         <v>11</v>
@@ -509,7 +500,7 @@
     </row>
     <row r="13" outlineLevel="1">
       <c r="A13" t="n" s="5">
-        <v>6.135272997198626E-6</v>
+        <v>2.391272801105515E-6</v>
       </c>
       <c r="B13" t="s" s="4">
         <v>25</v>
@@ -524,7 +515,7 @@
         <v>35.0</v>
       </c>
       <c r="F13" t="n" s="7">
-        <v>0.0</v>
+        <v>8.0</v>
       </c>
       <c r="G13" t="s" s="4">
         <v>11</v>
@@ -535,105 +526,27 @@
     </row>
     <row r="14" outlineLevel="1">
       <c r="A14" t="n" s="5">
-        <v>3.2890682177821873E-6</v>
+        <v>5.803636327073036E-7</v>
       </c>
       <c r="B14" t="s" s="4">
         <v>26</v>
       </c>
       <c r="C14" t="n" s="2">
-        <v>49.45454406738281</v>
+        <v>4.3636369705200195</v>
       </c>
       <c r="D14" t="n" s="2">
-        <v>17.30908966064453</v>
+        <v>1.5272730588912964</v>
       </c>
       <c r="E14" t="n" s="7">
+        <v>2.0</v>
+      </c>
+      <c r="F14" t="n" s="7">
         <v>1.0</v>
       </c>
-      <c r="F14" t="n" s="7">
-        <v>0.0</v>
-      </c>
       <c r="G14" t="s" s="4">
         <v>11</v>
       </c>
       <c r="H14" t="s" s="4">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" outlineLevel="1">
-      <c r="A15" t="n" s="5">
-        <v>2.9988564165250864E-6</v>
-      </c>
-      <c r="B15" t="s" s="4">
-        <v>27</v>
-      </c>
-      <c r="C15" t="n" s="2">
-        <v>45.09090805053711</v>
-      </c>
-      <c r="D15" t="n" s="2">
-        <v>15.443017959594727</v>
-      </c>
-      <c r="E15" t="n" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="F15" t="n" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="G15" t="s" s="4">
-        <v>11</v>
-      </c>
-      <c r="H15" t="s" s="4">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" outlineLevel="1">
-      <c r="A16" t="n" s="5">
-        <v>2.757013135123998E-6</v>
-      </c>
-      <c r="B16" t="s" s="4">
-        <v>28</v>
-      </c>
-      <c r="C16" t="n" s="2">
-        <v>41.45454406738281</v>
-      </c>
-      <c r="D16" t="n" s="2">
-        <v>14.5090913772583</v>
-      </c>
-      <c r="E16" t="n" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="F16" t="n" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="G16" t="s" s="4">
-        <v>11</v>
-      </c>
-      <c r="H16" t="s" s="4">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" outlineLevel="1">
-      <c r="A17" t="n" s="5">
-        <v>7.584046102238062E-7</v>
-      </c>
-      <c r="B17" t="s" s="4">
-        <v>29</v>
-      </c>
-      <c r="C17" t="n" s="2">
-        <v>4.3636369705200195</v>
-      </c>
-      <c r="D17" t="n" s="2">
-        <v>1.5272730588912964</v>
-      </c>
-      <c r="E17" t="n" s="7">
-        <v>2.0</v>
-      </c>
-      <c r="F17" t="n" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="G17" t="s" s="4">
-        <v>11</v>
-      </c>
-      <c r="H17" t="s" s="4">
         <v>12</v>
       </c>
     </row>

</xml_diff>